<commit_message>
# ISM LIBRARIES ISM
## Where :
All

## Description :
Setup back the new version

## How
-
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/txt/access.xlsx
+++ b/src/main/webapp/resources/txt/access.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="755">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="760">
   <si>
     <t>ID</t>
   </si>
@@ -2291,6 +2291,21 @@
   </si>
   <si>
     <t>IsGourou</t>
+  </si>
+  <si>
+    <t>SNC_REQUEST_CL</t>
+  </si>
+  <si>
+    <t>Cloture Action SMQ Request</t>
+  </si>
+  <si>
+    <t>Clôturer</t>
+  </si>
+  <si>
+    <t>ncRequestCloture</t>
+  </si>
+  <si>
+    <t>Permet de clôturer une demande de non-conformité</t>
   </si>
 </sst>
 </file>
@@ -2385,7 +2400,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -2403,6 +2418,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4307,13 +4325,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R121"/>
+  <dimension ref="A1:R122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="P106" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G48" sqref="G48"/>
+      <selection pane="bottomRight" activeCell="R112" sqref="R112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4325,7 +4343,7 @@
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="87.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.140625" customWidth="1"/>
     <col min="10" max="10" width="70.5703125" customWidth="1"/>
     <col min="11" max="12" width="36.5703125" customWidth="1"/>
@@ -4334,7 +4352,7 @@
     <col min="15" max="15" width="10.140625" customWidth="1"/>
     <col min="16" max="16" width="27.140625" customWidth="1"/>
     <col min="17" max="17" width="29.5703125" customWidth="1"/>
-    <col min="18" max="18" width="42.42578125" customWidth="1"/>
+    <col min="18" max="18" width="68.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4391,7 +4409,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="203.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -9738,7 +9756,7 @@
         <v>95</v>
       </c>
       <c r="J61" s="9" t="str">
-        <f t="shared" ref="J61:J121" si="8">"&lt;security-constraint&gt;
+        <f t="shared" ref="J61:J122" si="8">"&lt;security-constraint&gt;
         &lt;display-name&gt;" &amp; D61 &amp; " Security onstraint&lt;/display-name&gt;
         &lt;web-resource-collection&gt;
             &lt;web-resource-name&gt;" &amp; D61 &amp; " Web Security&lt;/web-resource-name&gt;
@@ -9766,7 +9784,7 @@
     &lt;/security-constraint&gt;</v>
       </c>
       <c r="K61" s="9" t="str">
-        <f t="shared" ref="K61:K121" si="9">"&lt;security-role&gt;
+        <f t="shared" ref="K61:K122" si="9">"&lt;security-role&gt;
 &lt;role-name&gt;" &amp; C61 &amp; "&lt;/role-name&gt;
 &lt;/security-role&gt;"</f>
         <v>&lt;security-role&gt;
@@ -9774,7 +9792,7 @@
 &lt;/security-role&gt;</v>
       </c>
       <c r="L61" s="6" t="str">
-        <f t="shared" ref="L61:L121" si="10">"&lt;security-role-mapping&gt;
+        <f t="shared" ref="L61:L122" si="10">"&lt;security-role-mapping&gt;
     &lt;role-name&gt;" &amp; C61 &amp; "&lt;/role-name&gt;
     &lt;group-name&gt;" &amp; C61 &amp; "&lt;/group-name&gt;
   &lt;/security-role-mapping&gt;"</f>
@@ -9784,7 +9802,7 @@
   &lt;/security-role-mapping&gt;</v>
       </c>
       <c r="M61" s="9" t="str">
-        <f t="shared" ref="M61:M121" si="11">F61 &amp; "_Name=" &amp; E61 &amp; "
+        <f t="shared" ref="M61:M122" si="11">F61 &amp; "_Name=" &amp; E61 &amp; "
 " &amp; F61 &amp; "_Path=" &amp; B61 &amp; "
 " &amp; F61 &amp; "_RoleName=" &amp; C61 &amp; "
 " &amp; F61 &amp; "_Description=" &amp; G61 &amp; CHAR(10)</f>
@@ -9795,7 +9813,7 @@
 </v>
       </c>
       <c r="N61" s="9" t="str">
-        <f t="shared" ref="N61:N121" si="12">"CheckboxTreeNode node" &amp; REPLACE(F61,1,1,UPPER(LEFT(F61,1))) &amp; " = new CheckboxTreeNode(new CtrlAccess(ResourceBundle.getBundle(JsfUtil.SECURITY).getString(""" &amp; F61 &amp; "_Name""),
+        <f t="shared" ref="N61:N122" si="12">"CheckboxTreeNode node" &amp; REPLACE(F61,1,1,UPPER(LEFT(F61,1))) &amp; " = new CheckboxTreeNode(new CtrlAccess(ResourceBundle.getBundle(JsfUtil.SECURITY).getString(""" &amp; F61 &amp; "_Name""),
                 ResourceBundle.getBundle(JsfUtil.SECURITY).getString("""  &amp; F61 &amp; "_RoleName""),
                 ResourceBundle.getBundle(JsfUtil.SECURITY).getString("""  &amp; F61 &amp; "_Path""""),
                 ResourceBundle.getBundle(JsfUtil.SECURITY).getString("""  &amp; F61 &amp; "_Description"""")),
@@ -9811,7 +9829,7 @@
         <v>0</v>
       </c>
       <c r="P61" s="6" t="str">
-        <f t="shared" ref="P61:P121" si="13">"INSERT INTO `ism`.`ism_role` (`role`, `rolename`) VALUES ('" &amp; C61 &amp; "', '" &amp; D61 &amp;"');"</f>
+        <f t="shared" ref="P61:P122" si="13">"INSERT INTO `ism`.`ism_role` (`role`, `rolename`) VALUES ('" &amp; C61 &amp; "', '" &amp; D61 &amp;"');"</f>
         <v>INSERT INTO `ism`.`ism_role` (`role`, `rolename`) VALUES ('HR_MANAGER', 'HR. Manager');</v>
       </c>
       <c r="Q61" s="11" t="str">
@@ -9819,7 +9837,7 @@
         <v>INSERT INTO `ism`.`staff_group_def_role` (`stgdr_company`, `stgdr_group_def`, `stgdr_role`, `stgdr_activated`, `stgdr_created`) VALUES ('39', 'GOUROU', 'HR_MANAGER', 1, NOW()),('39', 'ADMIN', 'HR_MANAGER', 1, NOW());</v>
       </c>
       <c r="R61" s="9" t="str">
-        <f t="shared" ref="R61:R121" si="14">"&lt;br /&gt;
+        <f t="shared" ref="R61:R122" si="14">"&lt;br /&gt;
  &lt;h:outputText value=""User in role " &amp; C61 &amp; " : #{request.isUserInRole('" &amp; C61 &amp; "')}"" /&gt;"</f>
         <v>&lt;br /&gt;
  &lt;h:outputText value="User in role HR_MANAGER : #{request.isUserInRole('HR_MANAGER')}" /&gt;</v>
@@ -9905,7 +9923,7 @@
         <v>INSERT INTO `ism`.`ism_role` (`role`, `rolename`) VALUES ('HR_MANAGER_C', 'Create HR. Manager');</v>
       </c>
       <c r="Q62" s="11" t="str">
-        <f t="shared" ref="Q62:Q121" si="15">IF(O62=0,"INSERT INTO `ism`.`staff_group_def_role` (`stgdr_company`, `stgdr_group_def`, `stgdr_role`, `stgdr_activated`, `stgdr_created`) VALUES ('39', 'GOUROU', '" &amp; C62 &amp; "', 1, NOW()),('39', 'ADMIN', '" &amp; C62 &amp; "', 1, NOW());","INSERT INTO `ism`.`staff_group_def_role` (`stgdr_company`, `stgdr_group_def`, `stgdr_role`, `stgdr_activated`, `stgdr_created`) VALUES ('39', 'GOUROU', '" &amp; C62 &amp; "', 1, NOW());")</f>
+        <f t="shared" ref="Q62:Q122" si="15">IF(O62=0,"INSERT INTO `ism`.`staff_group_def_role` (`stgdr_company`, `stgdr_group_def`, `stgdr_role`, `stgdr_activated`, `stgdr_created`) VALUES ('39', 'GOUROU', '" &amp; C62 &amp; "', 1, NOW()),('39', 'ADMIN', '" &amp; C62 &amp; "', 1, NOW());","INSERT INTO `ism`.`staff_group_def_role` (`stgdr_company`, `stgdr_group_def`, `stgdr_role`, `stgdr_activated`, `stgdr_created`) VALUES ('39', 'GOUROU', '" &amp; C62 &amp; "', 1, NOW());")</f>
         <v>INSERT INTO `ism`.`staff_group_def_role` (`stgdr_company`, `stgdr_group_def`, `stgdr_role`, `stgdr_activated`, `stgdr_created`) VALUES ('39', 'GOUROU', 'HR_MANAGER_C', 1, NOW()),('39', 'ADMIN', 'HR_MANAGER_C', 1, NOW());</v>
       </c>
       <c r="R62" s="9" t="str">
@@ -14188,7 +14206,7 @@
  &lt;h:outputText value="User in role SNC_REQUEST_R : #{request.isUserInRole('SNC_REQUEST_R')}" /&gt;</v>
       </c>
     </row>
-    <row r="111" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="2" t="s">
         <v>375</v>
@@ -14277,33 +14295,147 @@
  &lt;h:outputText value="User in role SNC_REQUEST_VA : #{request.isUserInRole('SNC_REQUEST_VA')}" /&gt;</v>
       </c>
     </row>
-    <row r="112" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="4"/>
-      <c r="B112" s="4" t="s">
-        <v>363</v>
-      </c>
-      <c r="C112" s="4" t="s">
-        <v>368</v>
-      </c>
-      <c r="D112" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="E112" s="4" t="s">
-        <v>671</v>
-      </c>
-      <c r="F112" s="4" t="s">
-        <v>539</v>
-      </c>
-      <c r="G112" s="4" t="s">
-        <v>738</v>
-      </c>
-      <c r="H112" s="4" t="s">
-        <v>57</v>
+    <row r="112" spans="1:18" ht="240" x14ac:dyDescent="0.25">
+      <c r="A112" s="2"/>
+      <c r="B112" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C112" s="8" t="s">
+        <v>755</v>
+      </c>
+      <c r="D112" s="8" t="s">
+        <v>756</v>
+      </c>
+      <c r="E112" s="8" t="s">
+        <v>757</v>
+      </c>
+      <c r="F112" s="8" t="s">
+        <v>758</v>
+      </c>
+      <c r="G112" s="8" t="s">
+        <v>759</v>
+      </c>
+      <c r="H112" s="8" t="s">
+        <v>531</v>
       </c>
       <c r="I112" t="s">
         <v>95</v>
       </c>
       <c r="J112" s="9" t="str">
+        <f t="shared" ref="J112" si="16">"&lt;security-constraint&gt;
+        &lt;display-name&gt;" &amp; D112 &amp; " Security onstraint&lt;/display-name&gt;
+        &lt;web-resource-collection&gt;
+            &lt;web-resource-name&gt;" &amp; D112 &amp; " Web Security&lt;/web-resource-name&gt;
+            &lt;url-pattern&gt;" &amp; B112 &amp; "&lt;/url-pattern&gt;
+        &lt;/web-resource-collection&gt;
+        &lt;auth-constraint&gt;
+            &lt;role-name&gt;" &amp; C112 &amp; "&lt;/role-name&gt;
+        &lt;/auth-constraint&gt;
+        &lt;user-data-constraint&gt;
+            &lt;transport-guarantee&gt;" &amp; I112 &amp; "&lt;/transport-guarantee&gt;
+        &lt;/user-data-constraint&gt;
+    &lt;/security-constraint&gt;"</f>
+        <v>&lt;security-constraint&gt;
+        &lt;display-name&gt;Cloture Action SMQ Request Security onstraint&lt;/display-name&gt;
+        &lt;web-resource-collection&gt;
+            &lt;web-resource-name&gt;Cloture Action SMQ Request Web Security&lt;/web-resource-name&gt;
+            &lt;url-pattern&gt;/faces/company/smq/nc/Request/View.xhtml&lt;/url-pattern&gt;
+        &lt;/web-resource-collection&gt;
+        &lt;auth-constraint&gt;
+            &lt;role-name&gt;SNC_REQUEST_CL&lt;/role-name&gt;
+        &lt;/auth-constraint&gt;
+        &lt;user-data-constraint&gt;
+            &lt;transport-guarantee&gt;CONFIDENTIAL&lt;/transport-guarantee&gt;
+        &lt;/user-data-constraint&gt;
+    &lt;/security-constraint&gt;</v>
+      </c>
+      <c r="K112" s="9" t="str">
+        <f t="shared" ref="K112" si="17">"&lt;security-role&gt;
+&lt;role-name&gt;" &amp; C112 &amp; "&lt;/role-name&gt;
+&lt;/security-role&gt;"</f>
+        <v>&lt;security-role&gt;
+&lt;role-name&gt;SNC_REQUEST_CL&lt;/role-name&gt;
+&lt;/security-role&gt;</v>
+      </c>
+      <c r="L112" s="12" t="str">
+        <f>"&lt;security-role-mapping&gt;
+    &lt;role-name&gt;" &amp; C112 &amp; "&lt;/role-name&gt;
+    &lt;group-name&gt;" &amp; C112 &amp; "&lt;/group-name&gt;
+  &lt;/security-role-mapping&gt;"</f>
+        <v>&lt;security-role-mapping&gt;
+    &lt;role-name&gt;SNC_REQUEST_CL&lt;/role-name&gt;
+    &lt;group-name&gt;SNC_REQUEST_CL&lt;/group-name&gt;
+  &lt;/security-role-mapping&gt;</v>
+      </c>
+      <c r="M112" s="9" t="str">
+        <f t="shared" ref="M112" si="18">F112 &amp; "_Name=" &amp; E112 &amp; "
+" &amp; F112 &amp; "_Path=" &amp; B112 &amp; "
+" &amp; F112 &amp; "_RoleName=" &amp; C112 &amp; "
+" &amp; F112 &amp; "_Description=" &amp; G112 &amp; CHAR(10)</f>
+        <v xml:space="preserve">ncRequestCloture_Name=Clôturer
+ncRequestCloture_Path=/faces/company/smq/nc/Request/View.xhtml
+ncRequestCloture_RoleName=SNC_REQUEST_CL
+ncRequestCloture_Description=Permet de clôturer une demande de non-conformité
+</v>
+      </c>
+      <c r="N112" s="9" t="str">
+        <f t="shared" ref="N112" si="19">"CheckboxTreeNode node" &amp; REPLACE(F112,1,1,UPPER(LEFT(F112,1))) &amp; " = new CheckboxTreeNode(new CtrlAccess(ResourceBundle.getBundle(JsfUtil.SECURITY).getString(""" &amp; F112 &amp; "_Name""),
+                ResourceBundle.getBundle(JsfUtil.SECURITY).getString("""  &amp; F112 &amp; "_RoleName""),
+                ResourceBundle.getBundle(JsfUtil.SECURITY).getString("""  &amp; F112 &amp; "_Path""""),
+                ResourceBundle.getBundle(JsfUtil.SECURITY).getString("""  &amp; F112 &amp; "_Description"""")),
+                node" &amp; REPLACE(H112,1,1,UPPER(LEFT(H112,1))) &amp; ");" &amp; CHAR(10) &amp; """"</f>
+        <v>CheckboxTreeNode nodeNcRequestCloture = new CheckboxTreeNode(new CtrlAccess(ResourceBundle.getBundle(JsfUtil.SECURITY).getString("ncRequestCloture_Name"),
+                ResourceBundle.getBundle(JsfUtil.SECURITY).getString("ncRequestCloture_RoleName"),
+                ResourceBundle.getBundle(JsfUtil.SECURITY).getString("ncRequestCloture_Path""),
+                ResourceBundle.getBundle(JsfUtil.SECURITY).getString("ncRequestCloture_Description"")),
+                nodeNcRequest);
+"</v>
+      </c>
+      <c r="O112" s="9">
+        <v>0</v>
+      </c>
+      <c r="P112" s="9" t="str">
+        <f t="shared" ref="P112" si="20">"INSERT INTO `ism`.`ism_role` (`role`, `rolename`) VALUES ('" &amp; C112 &amp; "', '" &amp; D112 &amp;"');"</f>
+        <v>INSERT INTO `ism`.`ism_role` (`role`, `rolename`) VALUES ('SNC_REQUEST_CL', 'Cloture Action SMQ Request');</v>
+      </c>
+      <c r="Q112" s="9" t="str">
+        <f t="shared" ref="Q112" si="21">IF(O112=0,"INSERT INTO `ism`.`staff_group_def_role` (`stgdr_company`, `stgdr_group_def`, `stgdr_role`, `stgdr_activated`, `stgdr_created`) VALUES ('39', 'GOUROU', '" &amp; C112 &amp; "', 1, NOW()),('39', 'ADMIN', '" &amp; C112 &amp; "', 1, NOW());","INSERT INTO `ism`.`staff_group_def_role` (`stgdr_company`, `stgdr_group_def`, `stgdr_role`, `stgdr_activated`, `stgdr_created`) VALUES ('39', 'GOUROU', '" &amp; C112 &amp; "', 1, NOW());")</f>
+        <v>INSERT INTO `ism`.`staff_group_def_role` (`stgdr_company`, `stgdr_group_def`, `stgdr_role`, `stgdr_activated`, `stgdr_created`) VALUES ('39', 'GOUROU', 'SNC_REQUEST_CL', 1, NOW()),('39', 'ADMIN', 'SNC_REQUEST_CL', 1, NOW());</v>
+      </c>
+      <c r="R112" s="9" t="str">
+        <f t="shared" ref="R112" si="22">"&lt;br /&gt;
+ &lt;h:outputText value=""User in role " &amp; C112 &amp; " : #{request.isUserInRole('" &amp; C112 &amp; "')}"" /&gt;"</f>
+        <v>&lt;br /&gt;
+ &lt;h:outputText value="User in role SNC_REQUEST_CL : #{request.isUserInRole('SNC_REQUEST_CL')}" /&gt;</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="4"/>
+      <c r="B113" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="F113" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="G113" s="4" t="s">
+        <v>738</v>
+      </c>
+      <c r="H113" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I113" t="s">
+        <v>95</v>
+      </c>
+      <c r="J113" s="9" t="str">
         <f t="shared" si="8"/>
         <v>&lt;security-constraint&gt;
         &lt;display-name&gt;SMQ Unite Security onstraint&lt;/display-name&gt;
@@ -14319,20 +14451,20 @@
         &lt;/user-data-constraint&gt;
     &lt;/security-constraint&gt;</v>
       </c>
-      <c r="K112" s="9" t="str">
+      <c r="K113" s="9" t="str">
         <f t="shared" si="9"/>
         <v>&lt;security-role&gt;
 &lt;role-name&gt;SNC_UNITE&lt;/role-name&gt;
 &lt;/security-role&gt;</v>
       </c>
-      <c r="L112" s="6" t="str">
+      <c r="L113" s="6" t="str">
         <f t="shared" si="10"/>
         <v>&lt;security-role-mapping&gt;
     &lt;role-name&gt;SNC_UNITE&lt;/role-name&gt;
     &lt;group-name&gt;SNC_UNITE&lt;/group-name&gt;
   &lt;/security-role-mapping&gt;</v>
       </c>
-      <c r="M112" s="9" t="str">
+      <c r="M113" s="9" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve">ncUnite_Name=Unité
 ncUnite_Path=/faces/company/smq/nc/Unite/*
@@ -14340,7 +14472,7 @@
 ncUnite_Description=Permet la gestion des unités de non conformités
 </v>
       </c>
-      <c r="N112" s="9" t="str">
+      <c r="N113" s="9" t="str">
         <f t="shared" si="12"/>
         <v>CheckboxTreeNode nodeNcUnite = new CheckboxTreeNode(new CtrlAccess(ResourceBundle.getBundle(JsfUtil.SECURITY).getString("ncUnite_Name"),
                 ResourceBundle.getBundle(JsfUtil.SECURITY).getString("ncUnite_RoleName"),
@@ -14349,50 +14481,50 @@
                 nodeNc);
 "</v>
       </c>
-      <c r="O112" s="9">
+      <c r="O113" s="9">
         <v>0</v>
       </c>
-      <c r="P112" s="6" t="str">
+      <c r="P113" s="6" t="str">
         <f t="shared" si="13"/>
         <v>INSERT INTO `ism`.`ism_role` (`role`, `rolename`) VALUES ('SNC_UNITE', 'SMQ Unite');</v>
       </c>
-      <c r="Q112" s="11" t="str">
+      <c r="Q113" s="11" t="str">
         <f t="shared" si="15"/>
         <v>INSERT INTO `ism`.`staff_group_def_role` (`stgdr_company`, `stgdr_group_def`, `stgdr_role`, `stgdr_activated`, `stgdr_created`) VALUES ('39', 'GOUROU', 'SNC_UNITE', 1, NOW()),('39', 'ADMIN', 'SNC_UNITE', 1, NOW());</v>
       </c>
-      <c r="R112" s="9" t="str">
+      <c r="R113" s="9" t="str">
         <f t="shared" si="14"/>
         <v>&lt;br /&gt;
  &lt;h:outputText value="User in role SNC_UNITE : #{request.isUserInRole('SNC_UNITE')}" /&gt;</v>
       </c>
     </row>
-    <row r="113" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="2"/>
-      <c r="B113" s="2" t="s">
+    <row r="114" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="2"/>
+      <c r="B114" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="C113" s="8" t="s">
+      <c r="C114" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="D113" s="8" t="s">
+      <c r="D114" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="E113" s="8" t="s">
+      <c r="E114" s="8" t="s">
         <v>651</v>
       </c>
-      <c r="F113" s="8" t="s">
+      <c r="F114" s="8" t="s">
         <v>540</v>
       </c>
-      <c r="G113" s="8" t="s">
+      <c r="G114" s="8" t="s">
         <v>739</v>
       </c>
-      <c r="H113" s="8" t="s">
+      <c r="H114" s="8" t="s">
         <v>539</v>
       </c>
-      <c r="I113" t="s">
+      <c r="I114" t="s">
         <v>95</v>
       </c>
-      <c r="J113" s="9" t="str">
+      <c r="J114" s="9" t="str">
         <f t="shared" si="8"/>
         <v>&lt;security-constraint&gt;
         &lt;display-name&gt;Create SMQ Unite Security onstraint&lt;/display-name&gt;
@@ -14408,20 +14540,20 @@
         &lt;/user-data-constraint&gt;
     &lt;/security-constraint&gt;</v>
       </c>
-      <c r="K113" s="9" t="str">
+      <c r="K114" s="9" t="str">
         <f t="shared" si="9"/>
         <v>&lt;security-role&gt;
 &lt;role-name&gt;SNC_UNITE_C&lt;/role-name&gt;
 &lt;/security-role&gt;</v>
       </c>
-      <c r="L113" s="6" t="str">
+      <c r="L114" s="6" t="str">
         <f t="shared" si="10"/>
         <v>&lt;security-role-mapping&gt;
     &lt;role-name&gt;SNC_UNITE_C&lt;/role-name&gt;
     &lt;group-name&gt;SNC_UNITE_C&lt;/group-name&gt;
   &lt;/security-role-mapping&gt;</v>
       </c>
-      <c r="M113" s="9" t="str">
+      <c r="M114" s="9" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve">ncUniteCreate_Name=Création
 ncUniteCreate_Path=/faces/company/smq/nc/Unite/Create.xhtml
@@ -14429,7 +14561,7 @@
 ncUniteCreate_Description=Permet la création d'une unité de non-conformité
 </v>
       </c>
-      <c r="N113" s="9" t="str">
+      <c r="N114" s="9" t="str">
         <f t="shared" si="12"/>
         <v>CheckboxTreeNode nodeNcUniteCreate = new CheckboxTreeNode(new CtrlAccess(ResourceBundle.getBundle(JsfUtil.SECURITY).getString("ncUniteCreate_Name"),
                 ResourceBundle.getBundle(JsfUtil.SECURITY).getString("ncUniteCreate_RoleName"),
@@ -14438,50 +14570,50 @@
                 nodeNcUnite);
 "</v>
       </c>
-      <c r="O113" s="9">
+      <c r="O114" s="9">
         <v>0</v>
       </c>
-      <c r="P113" s="6" t="str">
+      <c r="P114" s="6" t="str">
         <f t="shared" si="13"/>
         <v>INSERT INTO `ism`.`ism_role` (`role`, `rolename`) VALUES ('SNC_UNITE_C', 'Create SMQ Unite');</v>
       </c>
-      <c r="Q113" s="11" t="str">
+      <c r="Q114" s="11" t="str">
         <f t="shared" si="15"/>
         <v>INSERT INTO `ism`.`staff_group_def_role` (`stgdr_company`, `stgdr_group_def`, `stgdr_role`, `stgdr_activated`, `stgdr_created`) VALUES ('39', 'GOUROU', 'SNC_UNITE_C', 1, NOW()),('39', 'ADMIN', 'SNC_UNITE_C', 1, NOW());</v>
       </c>
-      <c r="R113" s="9" t="str">
+      <c r="R114" s="9" t="str">
         <f t="shared" si="14"/>
         <v>&lt;br /&gt;
  &lt;h:outputText value="User in role SNC_UNITE_C : #{request.isUserInRole('SNC_UNITE_C')}" /&gt;</v>
       </c>
     </row>
-    <row r="114" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="2"/>
-      <c r="B114" s="2" t="s">
+    <row r="115" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="2"/>
+      <c r="B115" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="C114" s="8" t="s">
+      <c r="C115" s="8" t="s">
         <v>370</v>
       </c>
-      <c r="D114" s="8" t="s">
+      <c r="D115" s="8" t="s">
         <v>436</v>
       </c>
-      <c r="E114" s="8" t="s">
+      <c r="E115" s="8" t="s">
         <v>645</v>
       </c>
-      <c r="F114" s="8" t="s">
+      <c r="F115" s="8" t="s">
         <v>541</v>
       </c>
-      <c r="G114" s="8" t="s">
+      <c r="G115" s="8" t="s">
         <v>740</v>
       </c>
-      <c r="H114" s="8" t="s">
+      <c r="H115" s="8" t="s">
         <v>539</v>
       </c>
-      <c r="I114" t="s">
+      <c r="I115" t="s">
         <v>95</v>
       </c>
-      <c r="J114" s="9" t="str">
+      <c r="J115" s="9" t="str">
         <f t="shared" si="8"/>
         <v>&lt;security-constraint&gt;
         &lt;display-name&gt;Edit SMQ Unite Security onstraint&lt;/display-name&gt;
@@ -14497,20 +14629,20 @@
         &lt;/user-data-constraint&gt;
     &lt;/security-constraint&gt;</v>
       </c>
-      <c r="K114" s="9" t="str">
+      <c r="K115" s="9" t="str">
         <f t="shared" si="9"/>
         <v>&lt;security-role&gt;
 &lt;role-name&gt;SNC_UNITE_E&lt;/role-name&gt;
 &lt;/security-role&gt;</v>
       </c>
-      <c r="L114" s="6" t="str">
+      <c r="L115" s="6" t="str">
         <f t="shared" si="10"/>
         <v>&lt;security-role-mapping&gt;
     &lt;role-name&gt;SNC_UNITE_E&lt;/role-name&gt;
     &lt;group-name&gt;SNC_UNITE_E&lt;/group-name&gt;
   &lt;/security-role-mapping&gt;</v>
       </c>
-      <c r="M114" s="9" t="str">
+      <c r="M115" s="9" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve">ncUniteEdit_Name=Edition
 ncUniteEdit_Path=/faces/company/smq/nc/Unite/Edit.xhtml
@@ -14518,7 +14650,7 @@
 ncUniteEdit_Description=Permet l'édition d'une unités de non conformités
 </v>
       </c>
-      <c r="N114" s="9" t="str">
+      <c r="N115" s="9" t="str">
         <f t="shared" si="12"/>
         <v>CheckboxTreeNode nodeNcUniteEdit = new CheckboxTreeNode(new CtrlAccess(ResourceBundle.getBundle(JsfUtil.SECURITY).getString("ncUniteEdit_Name"),
                 ResourceBundle.getBundle(JsfUtil.SECURITY).getString("ncUniteEdit_RoleName"),
@@ -14527,50 +14659,50 @@
                 nodeNcUnite);
 "</v>
       </c>
-      <c r="O114" s="9">
+      <c r="O115" s="9">
         <v>0</v>
       </c>
-      <c r="P114" s="6" t="str">
+      <c r="P115" s="6" t="str">
         <f t="shared" si="13"/>
         <v>INSERT INTO `ism`.`ism_role` (`role`, `rolename`) VALUES ('SNC_UNITE_E', 'Edit SMQ Unite');</v>
       </c>
-      <c r="Q114" s="11" t="str">
+      <c r="Q115" s="11" t="str">
         <f t="shared" si="15"/>
         <v>INSERT INTO `ism`.`staff_group_def_role` (`stgdr_company`, `stgdr_group_def`, `stgdr_role`, `stgdr_activated`, `stgdr_created`) VALUES ('39', 'GOUROU', 'SNC_UNITE_E', 1, NOW()),('39', 'ADMIN', 'SNC_UNITE_E', 1, NOW());</v>
       </c>
-      <c r="R114" s="9" t="str">
+      <c r="R115" s="9" t="str">
         <f t="shared" si="14"/>
         <v>&lt;br /&gt;
  &lt;h:outputText value="User in role SNC_UNITE_E : #{request.isUserInRole('SNC_UNITE_E')}" /&gt;</v>
       </c>
     </row>
-    <row r="115" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="2"/>
-      <c r="B115" s="2" t="s">
+    <row r="116" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="2"/>
+      <c r="B116" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="C115" s="8" t="s">
+      <c r="C116" s="8" t="s">
         <v>371</v>
       </c>
-      <c r="D115" s="8" t="s">
+      <c r="D116" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="E115" s="8" t="s">
+      <c r="E116" s="8" t="s">
         <v>646</v>
       </c>
-      <c r="F115" s="8" t="s">
+      <c r="F116" s="8" t="s">
         <v>542</v>
       </c>
-      <c r="G115" s="8" t="s">
+      <c r="G116" s="8" t="s">
         <v>741</v>
       </c>
-      <c r="H115" s="8" t="s">
+      <c r="H116" s="8" t="s">
         <v>539</v>
       </c>
-      <c r="I115" t="s">
+      <c r="I116" t="s">
         <v>95</v>
       </c>
-      <c r="J115" s="9" t="str">
+      <c r="J116" s="9" t="str">
         <f t="shared" si="8"/>
         <v>&lt;security-constraint&gt;
         &lt;display-name&gt;List SMQ Unite Security onstraint&lt;/display-name&gt;
@@ -14586,20 +14718,20 @@
         &lt;/user-data-constraint&gt;
     &lt;/security-constraint&gt;</v>
       </c>
-      <c r="K115" s="9" t="str">
+      <c r="K116" s="9" t="str">
         <f t="shared" si="9"/>
         <v>&lt;security-role&gt;
 &lt;role-name&gt;SNC_UNITE_L&lt;/role-name&gt;
 &lt;/security-role&gt;</v>
       </c>
-      <c r="L115" s="6" t="str">
+      <c r="L116" s="6" t="str">
         <f t="shared" si="10"/>
         <v>&lt;security-role-mapping&gt;
     &lt;role-name&gt;SNC_UNITE_L&lt;/role-name&gt;
     &lt;group-name&gt;SNC_UNITE_L&lt;/group-name&gt;
   &lt;/security-role-mapping&gt;</v>
       </c>
-      <c r="M115" s="9" t="str">
+      <c r="M116" s="9" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve">ncUniteList_Name=Lister
 ncUniteList_Path=/faces/company/smq/nc/Unite/List.xhtml
@@ -14607,7 +14739,7 @@
 ncUniteList_Description=Permet de visualiser la liste des unités de non-conformité
 </v>
       </c>
-      <c r="N115" s="9" t="str">
+      <c r="N116" s="9" t="str">
         <f t="shared" si="12"/>
         <v>CheckboxTreeNode nodeNcUniteList = new CheckboxTreeNode(new CtrlAccess(ResourceBundle.getBundle(JsfUtil.SECURITY).getString("ncUniteList_Name"),
                 ResourceBundle.getBundle(JsfUtil.SECURITY).getString("ncUniteList_RoleName"),
@@ -14616,50 +14748,50 @@
                 nodeNcUnite);
 "</v>
       </c>
-      <c r="O115" s="9">
+      <c r="O116" s="9">
         <v>0</v>
       </c>
-      <c r="P115" s="6" t="str">
+      <c r="P116" s="6" t="str">
         <f t="shared" si="13"/>
         <v>INSERT INTO `ism`.`ism_role` (`role`, `rolename`) VALUES ('SNC_UNITE_L', 'List SMQ Unite');</v>
       </c>
-      <c r="Q115" s="11" t="str">
+      <c r="Q116" s="11" t="str">
         <f t="shared" si="15"/>
         <v>INSERT INTO `ism`.`staff_group_def_role` (`stgdr_company`, `stgdr_group_def`, `stgdr_role`, `stgdr_activated`, `stgdr_created`) VALUES ('39', 'GOUROU', 'SNC_UNITE_L', 1, NOW()),('39', 'ADMIN', 'SNC_UNITE_L', 1, NOW());</v>
       </c>
-      <c r="R115" s="9" t="str">
+      <c r="R116" s="9" t="str">
         <f t="shared" si="14"/>
         <v>&lt;br /&gt;
  &lt;h:outputText value="User in role SNC_UNITE_L : #{request.isUserInRole('SNC_UNITE_L')}" /&gt;</v>
       </c>
     </row>
-    <row r="116" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="2"/>
-      <c r="B116" s="2" t="s">
+    <row r="117" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="2"/>
+      <c r="B117" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="C116" s="8" t="s">
+      <c r="C117" s="8" t="s">
         <v>372</v>
       </c>
-      <c r="D116" s="8" t="s">
+      <c r="D117" s="8" t="s">
         <v>438</v>
       </c>
-      <c r="E116" s="8" t="s">
+      <c r="E117" s="8" t="s">
         <v>647</v>
       </c>
-      <c r="F116" s="8" t="s">
+      <c r="F117" s="8" t="s">
         <v>543</v>
       </c>
-      <c r="G116" s="8" t="s">
+      <c r="G117" s="8" t="s">
         <v>742</v>
       </c>
-      <c r="H116" s="8" t="s">
+      <c r="H117" s="8" t="s">
         <v>539</v>
       </c>
-      <c r="I116" t="s">
+      <c r="I117" t="s">
         <v>95</v>
       </c>
-      <c r="J116" s="9" t="str">
+      <c r="J117" s="9" t="str">
         <f t="shared" si="8"/>
         <v>&lt;security-constraint&gt;
         &lt;display-name&gt;View SMQ Unite Security onstraint&lt;/display-name&gt;
@@ -14675,20 +14807,20 @@
         &lt;/user-data-constraint&gt;
     &lt;/security-constraint&gt;</v>
       </c>
-      <c r="K116" s="9" t="str">
+      <c r="K117" s="9" t="str">
         <f t="shared" si="9"/>
         <v>&lt;security-role&gt;
 &lt;role-name&gt;SNC_UNITE_V&lt;/role-name&gt;
 &lt;/security-role&gt;</v>
       </c>
-      <c r="L116" s="6" t="str">
+      <c r="L117" s="6" t="str">
         <f t="shared" si="10"/>
         <v>&lt;security-role-mapping&gt;
     &lt;role-name&gt;SNC_UNITE_V&lt;/role-name&gt;
     &lt;group-name&gt;SNC_UNITE_V&lt;/group-name&gt;
   &lt;/security-role-mapping&gt;</v>
       </c>
-      <c r="M116" s="9" t="str">
+      <c r="M117" s="9" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve">ncUniteView_Name=Visualiser
 ncUniteView_Path=/faces/company/smq/nc/Unite/View.xhtml
@@ -14696,7 +14828,7 @@
 ncUniteView_Description=Permet de visualiser le détail d'une unité de non-conformité
 </v>
       </c>
-      <c r="N116" s="9" t="str">
+      <c r="N117" s="9" t="str">
         <f t="shared" si="12"/>
         <v>CheckboxTreeNode nodeNcUniteView = new CheckboxTreeNode(new CtrlAccess(ResourceBundle.getBundle(JsfUtil.SECURITY).getString("ncUniteView_Name"),
                 ResourceBundle.getBundle(JsfUtil.SECURITY).getString("ncUniteView_RoleName"),
@@ -14705,50 +14837,50 @@
                 nodeNcUnite);
 "</v>
       </c>
-      <c r="O116" s="9">
+      <c r="O117" s="9">
         <v>0</v>
       </c>
-      <c r="P116" s="6" t="str">
+      <c r="P117" s="6" t="str">
         <f t="shared" si="13"/>
         <v>INSERT INTO `ism`.`ism_role` (`role`, `rolename`) VALUES ('SNC_UNITE_V', 'View SMQ Unite');</v>
       </c>
-      <c r="Q116" s="11" t="str">
+      <c r="Q117" s="11" t="str">
         <f t="shared" si="15"/>
         <v>INSERT INTO `ism`.`staff_group_def_role` (`stgdr_company`, `stgdr_group_def`, `stgdr_role`, `stgdr_activated`, `stgdr_created`) VALUES ('39', 'GOUROU', 'SNC_UNITE_V', 1, NOW()),('39', 'ADMIN', 'SNC_UNITE_V', 1, NOW());</v>
       </c>
-      <c r="R116" s="9" t="str">
+      <c r="R117" s="9" t="str">
         <f t="shared" si="14"/>
         <v>&lt;br /&gt;
  &lt;h:outputText value="User in role SNC_UNITE_V : #{request.isUserInRole('SNC_UNITE_V')}" /&gt;</v>
       </c>
     </row>
-    <row r="117" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="5"/>
-      <c r="B117" s="5" t="s">
+    <row r="118" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="5"/>
+      <c r="B118" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="C117" s="5" t="s">
+      <c r="C118" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="D117" s="5" t="s">
+      <c r="D118" s="5" t="s">
         <v>439</v>
       </c>
-      <c r="E117" s="5" t="s">
+      <c r="E118" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="F117" s="5" t="s">
+      <c r="F118" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G117" s="5" t="s">
+      <c r="G118" s="5" t="s">
         <v>743</v>
       </c>
-      <c r="H117" s="5" t="s">
+      <c r="H118" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="I117" t="s">
+      <c r="I118" t="s">
         <v>95</v>
       </c>
-      <c r="J117" s="9" t="str">
+      <c r="J118" s="9" t="str">
         <f t="shared" si="8"/>
         <v>&lt;security-constraint&gt;
         &lt;display-name&gt;SMQ processus Security onstraint&lt;/display-name&gt;
@@ -14764,20 +14896,20 @@
         &lt;/user-data-constraint&gt;
     &lt;/security-constraint&gt;</v>
       </c>
-      <c r="K117" s="9" t="str">
+      <c r="K118" s="9" t="str">
         <f t="shared" si="9"/>
         <v>&lt;security-role&gt;
 &lt;role-name&gt;S_PROCESSUS&lt;/role-name&gt;
 &lt;/security-role&gt;</v>
       </c>
-      <c r="L117" s="6" t="str">
+      <c r="L118" s="6" t="str">
         <f t="shared" si="10"/>
         <v>&lt;security-role-mapping&gt;
     &lt;role-name&gt;S_PROCESSUS&lt;/role-name&gt;
     &lt;group-name&gt;S_PROCESSUS&lt;/group-name&gt;
   &lt;/security-role-mapping&gt;</v>
       </c>
-      <c r="M117" s="9" t="str">
+      <c r="M118" s="9" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve">processus_Name=Processus
 processus_Path=/faces/company/smq/processus/*
@@ -14785,7 +14917,7 @@
 processus_Description=Permet la gestion des processus
 </v>
       </c>
-      <c r="N117" s="9" t="str">
+      <c r="N118" s="9" t="str">
         <f t="shared" si="12"/>
         <v>CheckboxTreeNode nodeProcessus = new CheckboxTreeNode(new CtrlAccess(ResourceBundle.getBundle(JsfUtil.SECURITY).getString("processus_Name"),
                 ResourceBundle.getBundle(JsfUtil.SECURITY).getString("processus_RoleName"),
@@ -14794,50 +14926,50 @@
                 nodeSMQ);
 "</v>
       </c>
-      <c r="O117" s="9">
+      <c r="O118" s="9">
         <v>0</v>
       </c>
-      <c r="P117" s="6" t="str">
+      <c r="P118" s="6" t="str">
         <f t="shared" si="13"/>
         <v>INSERT INTO `ism`.`ism_role` (`role`, `rolename`) VALUES ('S_PROCESSUS', 'SMQ processus');</v>
       </c>
-      <c r="Q117" s="11" t="str">
+      <c r="Q118" s="11" t="str">
         <f t="shared" si="15"/>
         <v>INSERT INTO `ism`.`staff_group_def_role` (`stgdr_company`, `stgdr_group_def`, `stgdr_role`, `stgdr_activated`, `stgdr_created`) VALUES ('39', 'GOUROU', 'S_PROCESSUS', 1, NOW()),('39', 'ADMIN', 'S_PROCESSUS', 1, NOW());</v>
       </c>
-      <c r="R117" s="9" t="str">
+      <c r="R118" s="9" t="str">
         <f t="shared" si="14"/>
         <v>&lt;br /&gt;
  &lt;h:outputText value="User in role S_PROCESSUS : #{request.isUserInRole('S_PROCESSUS')}" /&gt;</v>
       </c>
     </row>
-    <row r="118" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="2"/>
-      <c r="B118" s="2" t="s">
+    <row r="119" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="2"/>
+      <c r="B119" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="C118" s="8" t="s">
+      <c r="C119" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="D118" s="8" t="s">
+      <c r="D119" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="E118" s="8" t="s">
+      <c r="E119" s="8" t="s">
         <v>651</v>
       </c>
-      <c r="F118" s="8" t="s">
+      <c r="F119" s="8" t="s">
         <v>458</v>
       </c>
-      <c r="G118" s="8" t="s">
+      <c r="G119" s="8" t="s">
         <v>744</v>
       </c>
-      <c r="H118" s="8" t="s">
+      <c r="H119" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="I118" t="s">
+      <c r="I119" t="s">
         <v>95</v>
       </c>
-      <c r="J118" s="9" t="str">
+      <c r="J119" s="9" t="str">
         <f t="shared" si="8"/>
         <v>&lt;security-constraint&gt;
         &lt;display-name&gt;Create SMQ processus Security onstraint&lt;/display-name&gt;
@@ -14853,20 +14985,20 @@
         &lt;/user-data-constraint&gt;
     &lt;/security-constraint&gt;</v>
       </c>
-      <c r="K118" s="9" t="str">
+      <c r="K119" s="9" t="str">
         <f t="shared" si="9"/>
         <v>&lt;security-role&gt;
 &lt;role-name&gt;S_PROCESSUS_C&lt;/role-name&gt;
 &lt;/security-role&gt;</v>
       </c>
-      <c r="L118" s="6" t="str">
+      <c r="L119" s="6" t="str">
         <f t="shared" si="10"/>
         <v>&lt;security-role-mapping&gt;
     &lt;role-name&gt;S_PROCESSUS_C&lt;/role-name&gt;
     &lt;group-name&gt;S_PROCESSUS_C&lt;/group-name&gt;
   &lt;/security-role-mapping&gt;</v>
       </c>
-      <c r="M118" s="9" t="str">
+      <c r="M119" s="9" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve">processusCreate_Name=Création
 processusCreate_Path=/faces/company/smq/processus/Create.xhtml
@@ -14874,7 +15006,7 @@
 processusCreate_Description=Pemet la création d'un processus
 </v>
       </c>
-      <c r="N118" s="9" t="str">
+      <c r="N119" s="9" t="str">
         <f t="shared" si="12"/>
         <v>CheckboxTreeNode nodeProcessusCreate = new CheckboxTreeNode(new CtrlAccess(ResourceBundle.getBundle(JsfUtil.SECURITY).getString("processusCreate_Name"),
                 ResourceBundle.getBundle(JsfUtil.SECURITY).getString("processusCreate_RoleName"),
@@ -14883,50 +15015,50 @@
                 nodeProcessus);
 "</v>
       </c>
-      <c r="O118" s="9">
+      <c r="O119" s="9">
         <v>0</v>
       </c>
-      <c r="P118" s="6" t="str">
+      <c r="P119" s="6" t="str">
         <f t="shared" si="13"/>
         <v>INSERT INTO `ism`.`ism_role` (`role`, `rolename`) VALUES ('S_PROCESSUS_C', 'Create SMQ processus');</v>
       </c>
-      <c r="Q118" s="11" t="str">
+      <c r="Q119" s="11" t="str">
         <f t="shared" si="15"/>
         <v>INSERT INTO `ism`.`staff_group_def_role` (`stgdr_company`, `stgdr_group_def`, `stgdr_role`, `stgdr_activated`, `stgdr_created`) VALUES ('39', 'GOUROU', 'S_PROCESSUS_C', 1, NOW()),('39', 'ADMIN', 'S_PROCESSUS_C', 1, NOW());</v>
       </c>
-      <c r="R118" s="9" t="str">
+      <c r="R119" s="9" t="str">
         <f t="shared" si="14"/>
         <v>&lt;br /&gt;
  &lt;h:outputText value="User in role S_PROCESSUS_C : #{request.isUserInRole('S_PROCESSUS_C')}" /&gt;</v>
       </c>
     </row>
-    <row r="119" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="2"/>
-      <c r="B119" s="2" t="s">
+    <row r="120" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="2"/>
+      <c r="B120" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="C119" s="8" t="s">
+      <c r="C120" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="D119" s="8" t="s">
+      <c r="D120" s="8" t="s">
         <v>441</v>
       </c>
-      <c r="E119" s="8" t="s">
+      <c r="E120" s="8" t="s">
         <v>645</v>
       </c>
-      <c r="F119" s="8" t="s">
+      <c r="F120" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="G119" s="8" t="s">
+      <c r="G120" s="8" t="s">
         <v>745</v>
       </c>
-      <c r="H119" s="8" t="s">
+      <c r="H120" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="I119" t="s">
+      <c r="I120" t="s">
         <v>95</v>
       </c>
-      <c r="J119" s="9" t="str">
+      <c r="J120" s="9" t="str">
         <f t="shared" si="8"/>
         <v>&lt;security-constraint&gt;
         &lt;display-name&gt;Edit SMQ processus Security onstraint&lt;/display-name&gt;
@@ -14942,20 +15074,20 @@
         &lt;/user-data-constraint&gt;
     &lt;/security-constraint&gt;</v>
       </c>
-      <c r="K119" s="9" t="str">
+      <c r="K120" s="9" t="str">
         <f t="shared" si="9"/>
         <v>&lt;security-role&gt;
 &lt;role-name&gt;S_PROCESSUS_E&lt;/role-name&gt;
 &lt;/security-role&gt;</v>
       </c>
-      <c r="L119" s="6" t="str">
+      <c r="L120" s="6" t="str">
         <f t="shared" si="10"/>
         <v>&lt;security-role-mapping&gt;
     &lt;role-name&gt;S_PROCESSUS_E&lt;/role-name&gt;
     &lt;group-name&gt;S_PROCESSUS_E&lt;/group-name&gt;
   &lt;/security-role-mapping&gt;</v>
       </c>
-      <c r="M119" s="9" t="str">
+      <c r="M120" s="9" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve">processusEdit_Name=Edition
 processusEdit_Path=/faces/company/smq/processus/Edit.xhtml
@@ -14963,7 +15095,7 @@
 processusEdit_Description=Pemet l'édition d'un processus
 </v>
       </c>
-      <c r="N119" s="9" t="str">
+      <c r="N120" s="9" t="str">
         <f t="shared" si="12"/>
         <v>CheckboxTreeNode nodeProcessusEdit = new CheckboxTreeNode(new CtrlAccess(ResourceBundle.getBundle(JsfUtil.SECURITY).getString("processusEdit_Name"),
                 ResourceBundle.getBundle(JsfUtil.SECURITY).getString("processusEdit_RoleName"),
@@ -14972,50 +15104,50 @@
                 nodeProcessus);
 "</v>
       </c>
-      <c r="O119" s="9">
+      <c r="O120" s="9">
         <v>0</v>
       </c>
-      <c r="P119" s="6" t="str">
+      <c r="P120" s="6" t="str">
         <f t="shared" si="13"/>
         <v>INSERT INTO `ism`.`ism_role` (`role`, `rolename`) VALUES ('S_PROCESSUS_E', 'Edit SMQ processus');</v>
       </c>
-      <c r="Q119" s="11" t="str">
+      <c r="Q120" s="11" t="str">
         <f t="shared" si="15"/>
         <v>INSERT INTO `ism`.`staff_group_def_role` (`stgdr_company`, `stgdr_group_def`, `stgdr_role`, `stgdr_activated`, `stgdr_created`) VALUES ('39', 'GOUROU', 'S_PROCESSUS_E', 1, NOW()),('39', 'ADMIN', 'S_PROCESSUS_E', 1, NOW());</v>
       </c>
-      <c r="R119" s="9" t="str">
+      <c r="R120" s="9" t="str">
         <f t="shared" si="14"/>
         <v>&lt;br /&gt;
  &lt;h:outputText value="User in role S_PROCESSUS_E : #{request.isUserInRole('S_PROCESSUS_E')}" /&gt;</v>
       </c>
     </row>
-    <row r="120" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="2"/>
-      <c r="B120" s="2" t="s">
+    <row r="121" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="2"/>
+      <c r="B121" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="C120" s="8" t="s">
+      <c r="C121" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="D120" s="8" t="s">
+      <c r="D121" s="8" t="s">
         <v>442</v>
       </c>
-      <c r="E120" s="8" t="s">
+      <c r="E121" s="8" t="s">
         <v>646</v>
       </c>
-      <c r="F120" s="8" t="s">
+      <c r="F121" s="8" t="s">
         <v>545</v>
       </c>
-      <c r="G120" s="8" t="s">
+      <c r="G121" s="8" t="s">
         <v>746</v>
       </c>
-      <c r="H120" s="8" t="s">
+      <c r="H121" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="I120" t="s">
+      <c r="I121" t="s">
         <v>95</v>
       </c>
-      <c r="J120" s="9" t="str">
+      <c r="J121" s="9" t="str">
         <f t="shared" si="8"/>
         <v>&lt;security-constraint&gt;
         &lt;display-name&gt;List SMQ processus Security onstraint&lt;/display-name&gt;
@@ -15031,20 +15163,20 @@
         &lt;/user-data-constraint&gt;
     &lt;/security-constraint&gt;</v>
       </c>
-      <c r="K120" s="9" t="str">
+      <c r="K121" s="9" t="str">
         <f t="shared" si="9"/>
         <v>&lt;security-role&gt;
 &lt;role-name&gt;S_PROCESSUS_L&lt;/role-name&gt;
 &lt;/security-role&gt;</v>
       </c>
-      <c r="L120" s="6" t="str">
+      <c r="L121" s="6" t="str">
         <f t="shared" si="10"/>
         <v>&lt;security-role-mapping&gt;
     &lt;role-name&gt;S_PROCESSUS_L&lt;/role-name&gt;
     &lt;group-name&gt;S_PROCESSUS_L&lt;/group-name&gt;
   &lt;/security-role-mapping&gt;</v>
       </c>
-      <c r="M120" s="9" t="str">
+      <c r="M121" s="9" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve">processusList_Name=Lister
 processusList_Path=/faces/company/smq/processus/List.xhtml
@@ -15052,7 +15184,7 @@
 processusList_Description=Permet de visualiser la liste des processus
 </v>
       </c>
-      <c r="N120" s="9" t="str">
+      <c r="N121" s="9" t="str">
         <f t="shared" si="12"/>
         <v>CheckboxTreeNode nodeProcessusList = new CheckboxTreeNode(new CtrlAccess(ResourceBundle.getBundle(JsfUtil.SECURITY).getString("processusList_Name"),
                 ResourceBundle.getBundle(JsfUtil.SECURITY).getString("processusList_RoleName"),
@@ -15061,50 +15193,50 @@
                 nodeProcessus);
 "</v>
       </c>
-      <c r="O120" s="9">
+      <c r="O121" s="9">
         <v>0</v>
       </c>
-      <c r="P120" s="6" t="str">
+      <c r="P121" s="6" t="str">
         <f t="shared" si="13"/>
         <v>INSERT INTO `ism`.`ism_role` (`role`, `rolename`) VALUES ('S_PROCESSUS_L', 'List SMQ processus');</v>
       </c>
-      <c r="Q120" s="11" t="str">
+      <c r="Q121" s="11" t="str">
         <f t="shared" si="15"/>
         <v>INSERT INTO `ism`.`staff_group_def_role` (`stgdr_company`, `stgdr_group_def`, `stgdr_role`, `stgdr_activated`, `stgdr_created`) VALUES ('39', 'GOUROU', 'S_PROCESSUS_L', 1, NOW()),('39', 'ADMIN', 'S_PROCESSUS_L', 1, NOW());</v>
       </c>
-      <c r="R120" s="9" t="str">
+      <c r="R121" s="9" t="str">
         <f t="shared" si="14"/>
         <v>&lt;br /&gt;
  &lt;h:outputText value="User in role S_PROCESSUS_L : #{request.isUserInRole('S_PROCESSUS_L')}" /&gt;</v>
       </c>
     </row>
-    <row r="121" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="2"/>
-      <c r="B121" s="2" t="s">
+    <row r="122" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="2"/>
+      <c r="B122" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="C121" s="8" t="s">
+      <c r="C122" s="8" t="s">
         <v>326</v>
       </c>
-      <c r="D121" s="8" t="s">
+      <c r="D122" s="8" t="s">
         <v>443</v>
       </c>
-      <c r="E121" s="8" t="s">
+      <c r="E122" s="8" t="s">
         <v>647</v>
       </c>
-      <c r="F121" s="8" t="s">
+      <c r="F122" s="8" t="s">
         <v>546</v>
       </c>
-      <c r="G121" s="8" t="s">
+      <c r="G122" s="8" t="s">
         <v>747</v>
       </c>
-      <c r="H121" s="8" t="s">
+      <c r="H122" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="I121" t="s">
+      <c r="I122" t="s">
         <v>95</v>
       </c>
-      <c r="J121" s="9" t="str">
+      <c r="J122" s="9" t="str">
         <f t="shared" si="8"/>
         <v>&lt;security-constraint&gt;
         &lt;display-name&gt;View SMQ processus Security onstraint&lt;/display-name&gt;
@@ -15120,20 +15252,20 @@
         &lt;/user-data-constraint&gt;
     &lt;/security-constraint&gt;</v>
       </c>
-      <c r="K121" s="9" t="str">
+      <c r="K122" s="9" t="str">
         <f t="shared" si="9"/>
         <v>&lt;security-role&gt;
 &lt;role-name&gt;S_PROCESSUS_V&lt;/role-name&gt;
 &lt;/security-role&gt;</v>
       </c>
-      <c r="L121" s="6" t="str">
+      <c r="L122" s="6" t="str">
         <f t="shared" si="10"/>
         <v>&lt;security-role-mapping&gt;
     &lt;role-name&gt;S_PROCESSUS_V&lt;/role-name&gt;
     &lt;group-name&gt;S_PROCESSUS_V&lt;/group-name&gt;
   &lt;/security-role-mapping&gt;</v>
       </c>
-      <c r="M121" s="9" t="str">
+      <c r="M122" s="9" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve">processusView_Name=Visualiser
 processusView_Path=/faces/company/smq/processus/View.xhtml
@@ -15141,7 +15273,7 @@
 processusView_Description=Permet de visualiser le détail d'un processus
 </v>
       </c>
-      <c r="N121" s="9" t="str">
+      <c r="N122" s="9" t="str">
         <f t="shared" si="12"/>
         <v>CheckboxTreeNode nodeProcessusView = new CheckboxTreeNode(new CtrlAccess(ResourceBundle.getBundle(JsfUtil.SECURITY).getString("processusView_Name"),
                 ResourceBundle.getBundle(JsfUtil.SECURITY).getString("processusView_RoleName"),
@@ -15150,18 +15282,18 @@
                 nodeProcessus);
 "</v>
       </c>
-      <c r="O121" s="9">
+      <c r="O122" s="9">
         <v>0</v>
       </c>
-      <c r="P121" s="6" t="str">
+      <c r="P122" s="6" t="str">
         <f t="shared" si="13"/>
         <v>INSERT INTO `ism`.`ism_role` (`role`, `rolename`) VALUES ('S_PROCESSUS_V', 'View SMQ processus');</v>
       </c>
-      <c r="Q121" s="11" t="str">
+      <c r="Q122" s="11" t="str">
         <f t="shared" si="15"/>
         <v>INSERT INTO `ism`.`staff_group_def_role` (`stgdr_company`, `stgdr_group_def`, `stgdr_role`, `stgdr_activated`, `stgdr_created`) VALUES ('39', 'GOUROU', 'S_PROCESSUS_V', 1, NOW()),('39', 'ADMIN', 'S_PROCESSUS_V', 1, NOW());</v>
       </c>
-      <c r="R121" s="9" t="str">
+      <c r="R122" s="9" t="str">
         <f t="shared" si="14"/>
         <v>&lt;br /&gt;
  &lt;h:outputText value="User in role S_PROCESSUS_V : #{request.isUserInRole('S_PROCESSUS_V')}" /&gt;</v>

</xml_diff>